<commit_message>
Update with some datatypes
</commit_message>
<xml_diff>
--- a/Medical Clinic DB Schema.xlsx
+++ b/Medical Clinic DB Schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isse/Documents/College Documents/SP 2019 courses/DB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64C3849-76F3-6C48-AD6C-65D33FEEEF0F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F89E58-88AC-DC44-AE0A-7F8949AABFDA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="960" windowWidth="12280" windowHeight="19060" xr2:uid="{1D70DC5C-A134-D949-AA46-5DB15C9CAB9A}"/>
+    <workbookView xWindow="880" yWindow="960" windowWidth="26140" windowHeight="19060" xr2:uid="{1D70DC5C-A134-D949-AA46-5DB15C9CAB9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="90">
   <si>
     <t>Log_User_Name</t>
   </si>
@@ -273,6 +273,33 @@
   </si>
   <si>
     <t>Off_Addr_Zip</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>varchar(10)</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>varchar(50)</t>
+  </si>
+  <si>
+    <t>&lt;-Shouldn't it be date and not day?</t>
   </si>
 </sst>
 </file>
@@ -330,19 +357,17 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -659,431 +684,639 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{783F1F3F-01BC-BA45-A910-DC5E4D2C46B5}">
-  <dimension ref="A1:B88"/>
+  <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="18.1640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="6"/>
+    <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="B3" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="B4" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="B8" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="B9" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="B10" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="B11" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="B12" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="B13" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="B14" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="B15" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="B16" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="B17" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="B18" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="B19" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+      <c r="B23" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+      <c r="B24" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+      <c r="B25" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+      <c r="B26" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B29" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
+    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+      <c r="B30" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B31" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B34" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
+    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+      <c r="B35" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
+      <c r="B36" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
+      <c r="B37" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B38" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
+    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
+      <c r="B41" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
+      <c r="B42" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
+      <c r="B43" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
+      <c r="B44" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B45" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
+    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
+      <c r="B48" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
+      <c r="B49" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
+      <c r="B50" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="4" t="s">
+      <c r="B51" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="4" t="s">
+      <c r="B52" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
+      <c r="B53" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="4" t="s">
+      <c r="B54" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="4" t="s">
+      <c r="B55" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="4" t="s">
+      <c r="B56" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="4" t="s">
+      <c r="B57" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="4" t="s">
+      <c r="B58" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="4" t="s">
+      <c r="B59" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B60" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="s">
+    <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
+      <c r="B63" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
+      <c r="B64" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
+      <c r="B65" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
+      <c r="B66" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
+      <c r="B67" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
+      <c r="B68" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
+      <c r="B69" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
+      <c r="B70" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A72" s="4" t="s">
+      <c r="B71" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="4" t="s">
+      <c r="B72" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B73" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" s="4" t="s">
+    <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" s="4" t="s">
+      <c r="B76" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="4" t="s">
+    <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A79" s="4" t="s">
+    <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A80" s="4" t="s">
+    <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A81" s="4" t="s">
+    <row r="81" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A82" s="4" t="s">
+    <row r="82" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A83" s="4" t="s">
+    <row r="83" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" s="4" t="s">
+    <row r="84" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" s="4" t="s">
+      <c r="B84" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A86" s="4" t="s">
+      <c r="B85" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A87" s="4" t="s">
+      <c r="B86" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A88" s="4" t="s">
+      <c r="B87" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A88" s="3" t="s">
         <v>80</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Office Table Details
</commit_message>
<xml_diff>
--- a/Medical Clinic DB Schema.xlsx
+++ b/Medical Clinic DB Schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isse/Documents/College Documents/SP 2019 courses/DB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jw\Documents\School\U of H\Current Classes\COSC 3380 (Database)\Group Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F89E58-88AC-DC44-AE0A-7F8949AABFDA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD73D590-AB63-4346-BA12-88BDDA9CF00B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="960" windowWidth="26140" windowHeight="19060" xr2:uid="{1D70DC5C-A134-D949-AA46-5DB15C9CAB9A}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{1D70DC5C-A134-D949-AA46-5DB15C9CAB9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="90">
   <si>
     <t>Log_User_Name</t>
   </si>
@@ -354,20 +354,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -686,636 +685,656 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{783F1F3F-01BC-BA45-A910-DC5E4D2C46B5}">
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="6"/>
-    <col min="3" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="18.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="B4" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="B8" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="B9" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="B13" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="B15" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="B16" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="B17" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="B18" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="B22" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="B23" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" s="2" t="s">
+      <c r="B29" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="B30" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="B34" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+      <c r="B35" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
+      <c r="B36" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
+      <c r="B37" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="B41" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+      <c r="B42" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+      <c r="B43" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="5" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B48" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C48" s="2" t="s">
+      <c r="B48" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
+      <c r="B49" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B50" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
+      <c r="B50" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B51" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
+      <c r="B51" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B55" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
+      <c r="B55" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B56" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
+      <c r="B56" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B57" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
+      <c r="B57" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B58" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
+      <c r="B58" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B59" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
+      <c r="B59" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B63" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C63" s="2" t="s">
+      <c r="B63" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C63" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B64" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
+      <c r="B64" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B65" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="3" t="s">
+      <c r="B65" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B66" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="3" t="s">
+      <c r="B66" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B67" s="6" t="s">
+      <c r="B67" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="3" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B68" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="3" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B69" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="3" t="s">
+      <c r="B69" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B70" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="3" t="s">
+      <c r="B70" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B71" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A72" s="3" t="s">
+      <c r="B71" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B72" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="3" t="s">
+      <c r="B72" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B73" s="6" t="s">
+      <c r="B73" s="5" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" s="3" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B76" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C76" s="2" t="s">
+      <c r="B76" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C76" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" s="3" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="3" t="s">
+      <c r="B77" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A79" s="3" t="s">
+      <c r="B78" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A80" s="3" t="s">
+      <c r="B79" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A81" s="3" t="s">
+      <c r="B80" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A82" s="3" t="s">
+      <c r="B81" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
+      <c r="B82" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" s="3" t="s">
+      <c r="B83" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B84" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" s="3" t="s">
+      <c r="B84" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B85" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
+      <c r="B85" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B86" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
+      <c r="B86" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B87" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A88" s="3" t="s">
+      <c r="B87" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B88" s="6" t="s">
+      <c r="B88" s="5" t="s">
         <v>87</v>
       </c>
     </row>

</xml_diff>